<commit_message>
reporte: consolidado totales tipos depositos ok
</commit_message>
<xml_diff>
--- a/public/Reporte Consolidado Diario.xlsx
+++ b/public/Reporte Consolidado Diario.xlsx
@@ -1270,109 +1270,297 @@
       <c r="AW12" s="11"/>
     </row>
     <row r="13" spans="1:49">
-      <c r="A13" s="10"/>
+      <c r="A13" s="10">
+        <v>13</v>
+      </c>
       <c r="B13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="10"/>
-      <c r="Z13" s="10"/>
-      <c r="AA13" s="10"/>
-      <c r="AB13" s="10"/>
-      <c r="AC13" s="10"/>
-      <c r="AD13" s="10"/>
-      <c r="AE13" s="10"/>
-      <c r="AF13" s="10"/>
-      <c r="AG13" s="10"/>
-      <c r="AH13" s="10"/>
-      <c r="AI13" s="10"/>
-      <c r="AJ13" s="10"/>
-      <c r="AK13" s="10"/>
-      <c r="AL13" s="10"/>
-      <c r="AM13" s="10"/>
-      <c r="AN13" s="10"/>
-      <c r="AO13" s="10"/>
-      <c r="AP13" s="10"/>
-      <c r="AQ13" s="10"/>
-      <c r="AR13" s="10"/>
-      <c r="AS13" s="10"/>
-      <c r="AT13" s="10"/>
-      <c r="AU13" s="10"/>
-      <c r="AV13" s="10"/>
+      <c r="C13" s="10">
+        <v>14</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0</v>
+      </c>
+      <c r="M13" s="10">
+        <v>0</v>
+      </c>
+      <c r="N13" s="10">
+        <v>5</v>
+      </c>
+      <c r="O13" s="10">
+        <v>0</v>
+      </c>
+      <c r="P13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>0</v>
+      </c>
+      <c r="R13" s="10">
+        <v>0</v>
+      </c>
+      <c r="S13" s="10">
+        <v>0</v>
+      </c>
+      <c r="T13" s="10">
+        <v>0</v>
+      </c>
+      <c r="U13" s="10">
+        <v>0</v>
+      </c>
+      <c r="V13" s="10">
+        <v>0</v>
+      </c>
+      <c r="W13" s="10">
+        <v>0</v>
+      </c>
+      <c r="X13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AV13" s="10">
+        <v>5.0</v>
+      </c>
       <c r="AW13" s="10"/>
     </row>
     <row r="14" spans="1:49">
-      <c r="A14" s="10"/>
+      <c r="A14" s="10">
+        <v>14</v>
+      </c>
       <c r="B14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="10"/>
-      <c r="AB14" s="10"/>
-      <c r="AC14" s="10"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="10"/>
-      <c r="AF14" s="10"/>
-      <c r="AG14" s="10"/>
-      <c r="AH14" s="10"/>
-      <c r="AI14" s="10"/>
-      <c r="AJ14" s="10"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="10"/>
-      <c r="AM14" s="10"/>
-      <c r="AN14" s="10"/>
-      <c r="AO14" s="10"/>
-      <c r="AP14" s="10"/>
-      <c r="AQ14" s="10"/>
-      <c r="AR14" s="10"/>
-      <c r="AS14" s="10"/>
-      <c r="AT14" s="10"/>
-      <c r="AU14" s="10"/>
-      <c r="AV14" s="10"/>
+      <c r="C14" s="10">
+        <v>6</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
+        <v>2</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
+        <v>29</v>
+      </c>
+      <c r="K14" s="10">
+        <v>8</v>
+      </c>
+      <c r="L14" s="10">
+        <v>0</v>
+      </c>
+      <c r="M14" s="10">
+        <v>0</v>
+      </c>
+      <c r="N14" s="10">
+        <v>0</v>
+      </c>
+      <c r="O14" s="10">
+        <v>0</v>
+      </c>
+      <c r="P14" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>0</v>
+      </c>
+      <c r="R14" s="10">
+        <v>0</v>
+      </c>
+      <c r="S14" s="10">
+        <v>0</v>
+      </c>
+      <c r="T14" s="10">
+        <v>0</v>
+      </c>
+      <c r="U14" s="10">
+        <v>0</v>
+      </c>
+      <c r="V14" s="10">
+        <v>0</v>
+      </c>
+      <c r="W14" s="10">
+        <v>0</v>
+      </c>
+      <c r="X14" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="10">
+        <v>9.0</v>
+      </c>
       <c r="AW14" s="10"/>
     </row>
     <row r="15" spans="1:49">
@@ -2507,44 +2695,158 @@
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="10"/>
-      <c r="T37" s="10"/>
-      <c r="U37" s="10"/>
-      <c r="V37" s="10"/>
-      <c r="W37" s="10"/>
-      <c r="X37" s="10"/>
-      <c r="Y37" s="10"/>
-      <c r="Z37" s="10"/>
-      <c r="AA37" s="10"/>
-      <c r="AB37" s="10"/>
-      <c r="AC37" s="10"/>
-      <c r="AD37" s="10"/>
-      <c r="AE37" s="10"/>
-      <c r="AF37" s="10"/>
-      <c r="AG37" s="10"/>
-      <c r="AH37" s="10"/>
-      <c r="AI37" s="10"/>
-      <c r="AJ37" s="10"/>
-      <c r="AK37" s="10"/>
-      <c r="AL37" s="10"/>
-      <c r="AM37" s="10"/>
-      <c r="AN37" s="10"/>
-      <c r="AO37" s="10"/>
-      <c r="AP37" s="10"/>
-      <c r="AQ37" s="10"/>
-      <c r="AR37" s="10"/>
-      <c r="AS37" s="10"/>
-      <c r="AT37" s="10"/>
-      <c r="AU37" s="10"/>
+      <c r="J37" s="10">
+        <f>SUM(J13:J37)</f>
+        <v>29</v>
+      </c>
+      <c r="K37" s="10">
+        <f>SUM(K13:K37)</f>
+        <v>8</v>
+      </c>
+      <c r="L37" s="10">
+        <f>SUM(L13:L37)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="10">
+        <f>SUM(M13:M37)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="10">
+        <f>SUM(N13:N37)</f>
+        <v>5</v>
+      </c>
+      <c r="O37" s="10">
+        <f>SUM(O13:O37)</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="10">
+        <f>SUM(P13:P37)</f>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="10">
+        <f>SUM(Q13:Q37)</f>
+        <v>0</v>
+      </c>
+      <c r="R37" s="10">
+        <f>SUM(R13:R37)</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="10">
+        <f>SUM(S13:S37)</f>
+        <v>0</v>
+      </c>
+      <c r="T37" s="10">
+        <f>SUM(T13:T37)</f>
+        <v>0</v>
+      </c>
+      <c r="U37" s="10">
+        <f>SUM(U13:U37)</f>
+        <v>0</v>
+      </c>
+      <c r="V37" s="10">
+        <f>SUM(V13:V37)</f>
+        <v>0</v>
+      </c>
+      <c r="W37" s="10">
+        <f>SUM(W13:W37)</f>
+        <v>0</v>
+      </c>
+      <c r="X37" s="10">
+        <f>SUM(X13:X37)</f>
+        <v>0</v>
+      </c>
+      <c r="Y37" s="10">
+        <f>SUM(Y13:Y37)</f>
+        <v>0</v>
+      </c>
+      <c r="Z37" s="10">
+        <f>SUM(Z13:Z37)</f>
+        <v>0</v>
+      </c>
+      <c r="AA37" s="10">
+        <f>SUM(AA13:AA37)</f>
+        <v>0</v>
+      </c>
+      <c r="AB37" s="10">
+        <f>SUM(AB13:AB37)</f>
+        <v>0</v>
+      </c>
+      <c r="AC37" s="10">
+        <f>SUM(AC13:AC37)</f>
+        <v>0</v>
+      </c>
+      <c r="AD37" s="10">
+        <f>SUM(AD13:AD37)</f>
+        <v>0</v>
+      </c>
+      <c r="AE37" s="10">
+        <f>SUM(AE13:AE37)</f>
+        <v>0</v>
+      </c>
+      <c r="AF37" s="10">
+        <f>SUM(AF13:AF37)</f>
+        <v>0</v>
+      </c>
+      <c r="AG37" s="10">
+        <f>SUM(AG13:AG37)</f>
+        <v>0</v>
+      </c>
+      <c r="AH37" s="10">
+        <f>SUM(AH13:AH37)</f>
+        <v>0</v>
+      </c>
+      <c r="AI37" s="10">
+        <f>SUM(AI13:AI37)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ37" s="10">
+        <f>SUM(AJ13:AJ37)</f>
+        <v>0</v>
+      </c>
+      <c r="AK37" s="10">
+        <f>SUM(AK13:AK37)</f>
+        <v>0</v>
+      </c>
+      <c r="AL37" s="10">
+        <f>SUM(AL13:AL37)</f>
+        <v>0</v>
+      </c>
+      <c r="AM37" s="10">
+        <f>SUM(AM13:AM37)</f>
+        <v>0</v>
+      </c>
+      <c r="AN37" s="10">
+        <f>SUM(AN13:AN37)</f>
+        <v>0</v>
+      </c>
+      <c r="AO37" s="10">
+        <f>SUM(AO13:AO37)</f>
+        <v>0</v>
+      </c>
+      <c r="AP37" s="10">
+        <f>SUM(AP13:AP37)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ37" s="10">
+        <f>SUM(AQ13:AQ37)</f>
+        <v>0</v>
+      </c>
+      <c r="AR37" s="10">
+        <f>SUM(AR13:AR37)</f>
+        <v>0</v>
+      </c>
+      <c r="AS37" s="10">
+        <f>SUM(AS13:AS37)</f>
+        <v>0</v>
+      </c>
+      <c r="AT37" s="10">
+        <f>SUM(AT13:AT37)</f>
+        <v>0</v>
+      </c>
+      <c r="AU37" s="10">
+        <f>SUM(AU13:AU37)</f>
+        <v>0</v>
+      </c>
       <c r="AV37" s="10"/>
       <c r="AW37" s="10"/>
     </row>

</xml_diff>

<commit_message>
reportes: consolidado diario ok
</commit_message>
<xml_diff>
--- a/public/Reporte Consolidado Diario.xlsx
+++ b/public/Reporte Consolidado Diario.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>NTS N° 198 - MINSA/DIGESA-2023</t>
   </si>
@@ -149,10 +149,25 @@
     <t>Total</t>
   </si>
   <si>
-    <t>FERNANDEZ MAURICIO LORENZO</t>
-  </si>
-  <si>
     <t>SDFSDFDS</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Hora de ingreso</t>
+  </si>
+  <si>
+    <t>Hora de salida</t>
+  </si>
+  <si>
+    <t>FIRMA DEL SUPERVISOR O JEFE DE BRIGADA</t>
+  </si>
+  <si>
+    <t>Abreviaturas</t>
+  </si>
+  <si>
+    <t>Depósitos: en la columna: I(inspeccionado), P(positivo), TQ(tratamiento químico), TF(tratamiento fisico) o D(destruido), colocar el número de recipientes segun corresponda.</t>
   </si>
 </sst>
 </file>
@@ -160,7 +175,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -220,9 +235,36 @@
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="calibri"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,7 +275,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -265,11 +307,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="31">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -306,6 +494,34 @@
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="8" numFmtId="0" fillId="0" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="8" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="9" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="10" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="11" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="12" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="13" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="14" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="9" numFmtId="0" fillId="0" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,10 +857,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AW37"/>
+  <dimension ref="A1:AW49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A37" sqref="A37:AW37"/>
+      <selection activeCell="AK49" sqref="AK49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1273,35 +1489,35 @@
       <c r="AW12" s="11"/>
     </row>
     <row r="13" spans="1:49">
-      <c r="A13" s="10">
-        <v>13</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="10">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>2</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
         <v>1</v>
       </c>
-      <c r="E13" s="10">
-        <v>0</v>
-      </c>
-      <c r="F13" s="10">
-        <v>0</v>
-      </c>
-      <c r="G13" s="10">
-        <v>0</v>
-      </c>
-      <c r="H13" s="10">
-        <v>0</v>
-      </c>
-      <c r="I13" s="10">
-        <v>0</v>
-      </c>
       <c r="J13" s="10">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="K13" s="10">
         <v>0</v>
@@ -1313,10 +1529,10 @@
         <v>0</v>
       </c>
       <c r="N13" s="10">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O13" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P13" s="10">
         <v>0</v>
@@ -1415,155 +1631,59 @@
         <v>0</v>
       </c>
       <c r="AV13" s="10">
-        <v>5.0</v>
+        <v>9.0</v>
       </c>
       <c r="AW13" s="10"/>
     </row>
     <row r="14" spans="1:49">
-      <c r="A14" s="10">
-        <v>14</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="10">
-        <v>6</v>
-      </c>
-      <c r="D14" s="10">
-        <v>0</v>
-      </c>
-      <c r="E14" s="10">
-        <v>0</v>
-      </c>
-      <c r="F14" s="10">
-        <v>2</v>
-      </c>
-      <c r="G14" s="10">
-        <v>0</v>
-      </c>
-      <c r="H14" s="10">
-        <v>0</v>
-      </c>
-      <c r="I14" s="10">
-        <v>0</v>
-      </c>
-      <c r="J14" s="10">
-        <v>29</v>
-      </c>
-      <c r="K14" s="10">
-        <v>8</v>
-      </c>
-      <c r="L14" s="10">
-        <v>0</v>
-      </c>
-      <c r="M14" s="10">
-        <v>0</v>
-      </c>
-      <c r="N14" s="10">
-        <v>0</v>
-      </c>
-      <c r="O14" s="10">
-        <v>0</v>
-      </c>
-      <c r="P14" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="10">
-        <v>0</v>
-      </c>
-      <c r="R14" s="10">
-        <v>0</v>
-      </c>
-      <c r="S14" s="10">
-        <v>0</v>
-      </c>
-      <c r="T14" s="10">
-        <v>0</v>
-      </c>
-      <c r="U14" s="10">
-        <v>0</v>
-      </c>
-      <c r="V14" s="10">
-        <v>0</v>
-      </c>
-      <c r="W14" s="10">
-        <v>0</v>
-      </c>
-      <c r="X14" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AL14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AM14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AN14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AO14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AP14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AR14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AS14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AT14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AU14" s="10">
-        <v>0</v>
-      </c>
-      <c r="AV14" s="10">
-        <v>9.0</v>
-      </c>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="10"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="10"/>
+      <c r="AH14" s="10"/>
+      <c r="AI14" s="10"/>
+      <c r="AJ14" s="10"/>
+      <c r="AK14" s="10"/>
+      <c r="AL14" s="10"/>
+      <c r="AM14" s="10"/>
+      <c r="AN14" s="10"/>
+      <c r="AO14" s="10"/>
+      <c r="AP14" s="10"/>
+      <c r="AQ14" s="10"/>
+      <c r="AR14" s="10"/>
+      <c r="AS14" s="10"/>
+      <c r="AT14" s="10"/>
+      <c r="AU14" s="10"/>
+      <c r="AV14" s="10"/>
       <c r="AW14" s="10"/>
     </row>
     <row r="15" spans="1:49">
@@ -2689,192 +2809,678 @@
       <c r="AW36" s="10"/>
     </row>
     <row r="37" spans="1:49">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11">
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13">
         <f>SUM(D13:D36)</f>
-        <v>1</v>
-      </c>
-      <c r="E37" s="11">
+        <v>0</v>
+      </c>
+      <c r="E37" s="13">
         <f>SUM(E13:E36)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="13">
         <f>SUM(F13:F36)</f>
         <v>2</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="13">
         <f>SUM(G13:G36)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="11">
+      <c r="H37" s="13">
         <f>SUM(H13:H36)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="11">
+      <c r="I37" s="13">
         <f>SUM(I13:I36)</f>
-        <v>0</v>
-      </c>
-      <c r="J37" s="11">
+        <v>1</v>
+      </c>
+      <c r="J37" s="13">
         <f>SUM(J13:J36)</f>
         <v>29</v>
       </c>
-      <c r="K37" s="11">
+      <c r="K37" s="13">
         <f>SUM(K13:K36)</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="13">
+        <f>SUM(L13:L36)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="13">
+        <f>SUM(M13:M36)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="13">
+        <f>SUM(N13:N36)</f>
         <v>8</v>
       </c>
-      <c r="L37" s="11">
-        <f>SUM(L13:L36)</f>
-        <v>0</v>
-      </c>
-      <c r="M37" s="11">
-        <f>SUM(M13:M36)</f>
-        <v>0</v>
-      </c>
-      <c r="N37" s="11">
-        <f>SUM(N13:N36)</f>
-        <v>5</v>
-      </c>
-      <c r="O37" s="11">
+      <c r="O37" s="13">
         <f>SUM(O13:O36)</f>
-        <v>0</v>
-      </c>
-      <c r="P37" s="11">
+        <v>3</v>
+      </c>
+      <c r="P37" s="13">
         <f>SUM(P13:P36)</f>
         <v>0</v>
       </c>
-      <c r="Q37" s="11">
+      <c r="Q37" s="13">
         <f>SUM(Q13:Q36)</f>
         <v>0</v>
       </c>
-      <c r="R37" s="11">
+      <c r="R37" s="13">
         <f>SUM(R13:R36)</f>
         <v>0</v>
       </c>
-      <c r="S37" s="11">
+      <c r="S37" s="13">
         <f>SUM(S13:S36)</f>
         <v>0</v>
       </c>
-      <c r="T37" s="11">
+      <c r="T37" s="13">
         <f>SUM(T13:T36)</f>
         <v>0</v>
       </c>
-      <c r="U37" s="11">
+      <c r="U37" s="13">
         <f>SUM(U13:U36)</f>
         <v>0</v>
       </c>
-      <c r="V37" s="11">
+      <c r="V37" s="13">
         <f>SUM(V13:V36)</f>
         <v>0</v>
       </c>
-      <c r="W37" s="11">
+      <c r="W37" s="13">
         <f>SUM(W13:W36)</f>
         <v>0</v>
       </c>
-      <c r="X37" s="11">
+      <c r="X37" s="13">
         <f>SUM(X13:X36)</f>
         <v>0</v>
       </c>
-      <c r="Y37" s="11">
+      <c r="Y37" s="13">
         <f>SUM(Y13:Y36)</f>
         <v>0</v>
       </c>
-      <c r="Z37" s="11">
+      <c r="Z37" s="13">
         <f>SUM(Z13:Z36)</f>
         <v>0</v>
       </c>
-      <c r="AA37" s="11">
+      <c r="AA37" s="13">
         <f>SUM(AA13:AA36)</f>
         <v>0</v>
       </c>
-      <c r="AB37" s="11">
+      <c r="AB37" s="13">
         <f>SUM(AB13:AB36)</f>
         <v>0</v>
       </c>
-      <c r="AC37" s="11">
+      <c r="AC37" s="13">
         <f>SUM(AC13:AC36)</f>
         <v>0</v>
       </c>
-      <c r="AD37" s="11">
+      <c r="AD37" s="13">
         <f>SUM(AD13:AD36)</f>
         <v>0</v>
       </c>
-      <c r="AE37" s="11">
+      <c r="AE37" s="13">
         <f>SUM(AE13:AE36)</f>
         <v>0</v>
       </c>
-      <c r="AF37" s="11">
+      <c r="AF37" s="13">
         <f>SUM(AF13:AF36)</f>
         <v>0</v>
       </c>
-      <c r="AG37" s="11">
+      <c r="AG37" s="13">
         <f>SUM(AG13:AG36)</f>
         <v>0</v>
       </c>
-      <c r="AH37" s="11">
+      <c r="AH37" s="13">
         <f>SUM(AH13:AH36)</f>
         <v>0</v>
       </c>
-      <c r="AI37" s="11">
+      <c r="AI37" s="13">
         <f>SUM(AI13:AI36)</f>
         <v>0</v>
       </c>
-      <c r="AJ37" s="11">
+      <c r="AJ37" s="13">
         <f>SUM(AJ13:AJ36)</f>
         <v>0</v>
       </c>
-      <c r="AK37" s="11">
+      <c r="AK37" s="13">
         <f>SUM(AK13:AK36)</f>
         <v>0</v>
       </c>
-      <c r="AL37" s="11">
+      <c r="AL37" s="13">
         <f>SUM(AL13:AL36)</f>
         <v>0</v>
       </c>
-      <c r="AM37" s="11">
+      <c r="AM37" s="13">
         <f>SUM(AM13:AM36)</f>
         <v>0</v>
       </c>
-      <c r="AN37" s="11">
+      <c r="AN37" s="13">
         <f>SUM(AN13:AN36)</f>
         <v>0</v>
       </c>
-      <c r="AO37" s="11">
+      <c r="AO37" s="13">
         <f>SUM(AO13:AO36)</f>
         <v>0</v>
       </c>
-      <c r="AP37" s="11">
+      <c r="AP37" s="13">
         <f>SUM(AP13:AP36)</f>
         <v>0</v>
       </c>
-      <c r="AQ37" s="11">
+      <c r="AQ37" s="13">
         <f>SUM(AQ13:AQ36)</f>
         <v>0</v>
       </c>
-      <c r="AR37" s="11">
+      <c r="AR37" s="13">
         <f>SUM(AR13:AR36)</f>
         <v>0</v>
       </c>
-      <c r="AS37" s="11">
+      <c r="AS37" s="13">
         <f>SUM(AS13:AS36)</f>
         <v>0</v>
       </c>
-      <c r="AT37" s="11">
+      <c r="AT37" s="13">
         <f>SUM(AT13:AT36)</f>
         <v>0</v>
       </c>
-      <c r="AU37" s="11">
+      <c r="AU37" s="13">
         <f>SUM(AU13:AU36)</f>
         <v>0</v>
       </c>
-      <c r="AV37" s="11">
+      <c r="AV37" s="13">
         <f>SUM(AV13:AV36)</f>
-        <v>14</v>
-      </c>
-      <c r="AW37" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="AW37" s="13"/>
+    </row>
+    <row r="39" spans="1:49">
+      <c r="A39" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
+      <c r="V39" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="W39" s="15"/>
+      <c r="X39" s="15"/>
+      <c r="Y39" s="15"/>
+      <c r="Z39" s="15"/>
+      <c r="AA39" s="15"/>
+      <c r="AB39" s="15"/>
+      <c r="AC39" s="15"/>
+      <c r="AD39" s="15"/>
+      <c r="AE39" s="15"/>
+      <c r="AF39" s="15"/>
+      <c r="AG39" s="15"/>
+      <c r="AH39" s="15"/>
+      <c r="AI39" s="15"/>
+      <c r="AJ39" s="15"/>
+      <c r="AK39" s="15"/>
+      <c r="AL39" s="15"/>
+      <c r="AM39" s="15"/>
+      <c r="AN39" s="15"/>
+      <c r="AO39" s="15"/>
+      <c r="AP39" s="15"/>
+      <c r="AQ39" s="15"/>
+      <c r="AR39" s="15"/>
+      <c r="AS39" s="15"/>
+      <c r="AT39" s="15"/>
+      <c r="AU39" s="15"/>
+      <c r="AV39" s="15"/>
+      <c r="AW39" s="15"/>
+    </row>
+    <row r="40" spans="1:49">
+      <c r="V40" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:49">
+      <c r="V41" s="28"/>
+      <c r="W41" s="28"/>
+      <c r="X41" s="28"/>
+      <c r="Y41" s="28"/>
+      <c r="Z41" s="28"/>
+      <c r="AA41" s="28"/>
+      <c r="AB41" s="28"/>
+      <c r="AC41" s="28"/>
+      <c r="AD41" s="28"/>
+      <c r="AE41" s="28"/>
+      <c r="AF41" s="28"/>
+      <c r="AG41" s="28"/>
+      <c r="AH41" s="28"/>
+      <c r="AI41" s="28"/>
+      <c r="AJ41" s="28"/>
+      <c r="AK41" s="28"/>
+      <c r="AL41" s="28"/>
+      <c r="AM41" s="28"/>
+      <c r="AN41" s="28"/>
+      <c r="AO41" s="28"/>
+      <c r="AP41" s="28"/>
+      <c r="AQ41" s="28"/>
+      <c r="AR41" s="28"/>
+      <c r="AS41" s="28"/>
+      <c r="AT41" s="28"/>
+      <c r="AU41" s="28"/>
+      <c r="AV41" s="28"/>
+      <c r="AW41" s="28"/>
+    </row>
+    <row r="42" spans="1:49">
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="26"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="26"/>
+      <c r="P42" s="26"/>
+      <c r="Q42" s="26"/>
+      <c r="R42" s="26"/>
+      <c r="S42" s="26"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="29"/>
+      <c r="AB42" s="29"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="29"/>
+      <c r="AF42" s="29"/>
+      <c r="AG42" s="29"/>
+      <c r="AH42" s="29"/>
+      <c r="AI42" s="29"/>
+      <c r="AJ42" s="29"/>
+      <c r="AK42" s="29"/>
+      <c r="AL42" s="29"/>
+      <c r="AM42" s="29"/>
+      <c r="AN42" s="29"/>
+      <c r="AO42" s="29"/>
+      <c r="AP42" s="29"/>
+      <c r="AQ42" s="29"/>
+      <c r="AR42" s="29"/>
+      <c r="AS42" s="29"/>
+      <c r="AT42" s="29"/>
+      <c r="AU42" s="29"/>
+      <c r="AV42" s="29"/>
+      <c r="AW42" s="29"/>
+    </row>
+    <row r="43" spans="1:49">
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="26"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="26"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="19"/>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="19"/>
+      <c r="Z43" s="19"/>
+      <c r="AA43" s="19"/>
+      <c r="AB43" s="19"/>
+      <c r="AC43" s="19"/>
+      <c r="AD43" s="19"/>
+      <c r="AE43" s="19"/>
+      <c r="AF43" s="19"/>
+      <c r="AG43" s="19"/>
+      <c r="AH43" s="19"/>
+      <c r="AI43" s="19"/>
+      <c r="AJ43" s="19"/>
+      <c r="AK43" s="19"/>
+      <c r="AL43" s="19"/>
+      <c r="AM43" s="19"/>
+      <c r="AN43" s="19"/>
+      <c r="AO43" s="19"/>
+      <c r="AP43" s="19"/>
+      <c r="AQ43" s="19"/>
+      <c r="AR43" s="19"/>
+      <c r="AS43" s="19"/>
+      <c r="AT43" s="19"/>
+      <c r="AU43" s="19"/>
+      <c r="AV43" s="19"/>
+      <c r="AW43" s="22"/>
+    </row>
+    <row r="44" spans="1:49">
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="26"/>
+      <c r="N44" s="26"/>
+      <c r="O44" s="26"/>
+      <c r="P44" s="26"/>
+      <c r="Q44" s="26"/>
+      <c r="R44" s="26"/>
+      <c r="S44" s="26"/>
+      <c r="V44" s="17"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="20"/>
+      <c r="Y44" s="20"/>
+      <c r="Z44" s="20"/>
+      <c r="AA44" s="20"/>
+      <c r="AB44" s="20"/>
+      <c r="AC44" s="20"/>
+      <c r="AD44" s="20"/>
+      <c r="AE44" s="20"/>
+      <c r="AF44" s="20"/>
+      <c r="AG44" s="20"/>
+      <c r="AH44" s="20"/>
+      <c r="AI44" s="20"/>
+      <c r="AJ44" s="20"/>
+      <c r="AK44" s="20"/>
+      <c r="AL44" s="20"/>
+      <c r="AM44" s="20"/>
+      <c r="AN44" s="20"/>
+      <c r="AO44" s="20"/>
+      <c r="AP44" s="20"/>
+      <c r="AQ44" s="20"/>
+      <c r="AR44" s="20"/>
+      <c r="AS44" s="20"/>
+      <c r="AT44" s="20"/>
+      <c r="AU44" s="20"/>
+      <c r="AV44" s="20"/>
+      <c r="AW44" s="23"/>
+    </row>
+    <row r="45" spans="1:49">
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="26"/>
+      <c r="N45" s="26"/>
+      <c r="O45" s="26"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="26"/>
+      <c r="R45" s="26"/>
+      <c r="S45" s="26"/>
+      <c r="V45" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="W45" s="20"/>
+      <c r="X45" s="20"/>
+      <c r="Y45" s="20"/>
+      <c r="Z45" s="25"/>
+      <c r="AA45" s="25"/>
+      <c r="AB45" s="25"/>
+      <c r="AC45" s="25"/>
+      <c r="AD45" s="25"/>
+      <c r="AE45" s="20"/>
+      <c r="AF45" s="20"/>
+      <c r="AG45" s="20"/>
+      <c r="AH45" s="20"/>
+      <c r="AI45" s="20"/>
+      <c r="AJ45" s="20"/>
+      <c r="AK45" s="20"/>
+      <c r="AL45" s="20"/>
+      <c r="AM45" s="20"/>
+      <c r="AN45" s="20"/>
+      <c r="AO45" s="20"/>
+      <c r="AP45" s="20"/>
+      <c r="AQ45" s="20"/>
+      <c r="AR45" s="20"/>
+      <c r="AS45" s="20"/>
+      <c r="AT45" s="20"/>
+      <c r="AU45" s="20"/>
+      <c r="AV45" s="20"/>
+      <c r="AW45" s="23"/>
+    </row>
+    <row r="46" spans="1:49">
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="26"/>
+      <c r="N46" s="26"/>
+      <c r="O46" s="26"/>
+      <c r="P46" s="26"/>
+      <c r="Q46" s="26"/>
+      <c r="R46" s="26"/>
+      <c r="S46" s="26"/>
+      <c r="V46" s="17"/>
+      <c r="W46" s="20"/>
+      <c r="X46" s="20"/>
+      <c r="Y46" s="20"/>
+      <c r="Z46" s="20"/>
+      <c r="AA46" s="20"/>
+      <c r="AB46" s="20"/>
+      <c r="AC46" s="20"/>
+      <c r="AD46" s="20"/>
+      <c r="AE46" s="20"/>
+      <c r="AF46" s="20"/>
+      <c r="AG46" s="20"/>
+      <c r="AH46" s="20"/>
+      <c r="AI46" s="20"/>
+      <c r="AJ46" s="20"/>
+      <c r="AK46" s="20"/>
+      <c r="AL46" s="20"/>
+      <c r="AM46" s="20"/>
+      <c r="AN46" s="20"/>
+      <c r="AO46" s="20"/>
+      <c r="AP46" s="20"/>
+      <c r="AQ46" s="20"/>
+      <c r="AR46" s="20"/>
+      <c r="AS46" s="20"/>
+      <c r="AT46" s="20"/>
+      <c r="AU46" s="20"/>
+      <c r="AV46" s="20"/>
+      <c r="AW46" s="23"/>
+    </row>
+    <row r="47" spans="1:49">
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
+      <c r="N47" s="26"/>
+      <c r="O47" s="26"/>
+      <c r="P47" s="26"/>
+      <c r="Q47" s="26"/>
+      <c r="R47" s="26"/>
+      <c r="S47" s="26"/>
+      <c r="V47" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="W47" s="20"/>
+      <c r="X47" s="20"/>
+      <c r="Y47" s="20"/>
+      <c r="Z47" s="25"/>
+      <c r="AA47" s="25"/>
+      <c r="AB47" s="25"/>
+      <c r="AC47" s="25"/>
+      <c r="AD47" s="25"/>
+      <c r="AE47" s="20"/>
+      <c r="AF47" s="20"/>
+      <c r="AG47" s="20"/>
+      <c r="AH47" s="20"/>
+      <c r="AI47" s="20"/>
+      <c r="AJ47" s="20"/>
+      <c r="AK47" s="20"/>
+      <c r="AL47" s="20"/>
+      <c r="AM47" s="20"/>
+      <c r="AN47" s="20"/>
+      <c r="AO47" s="20"/>
+      <c r="AP47" s="20"/>
+      <c r="AQ47" s="20"/>
+      <c r="AR47" s="20"/>
+      <c r="AS47" s="20"/>
+      <c r="AT47" s="20"/>
+      <c r="AU47" s="20"/>
+      <c r="AV47" s="20"/>
+      <c r="AW47" s="23"/>
+    </row>
+    <row r="48" spans="1:49">
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="26"/>
+      <c r="N48" s="26"/>
+      <c r="O48" s="26"/>
+      <c r="P48" s="26"/>
+      <c r="Q48" s="26"/>
+      <c r="R48" s="26"/>
+      <c r="S48" s="26"/>
+      <c r="V48" s="17"/>
+      <c r="W48" s="20"/>
+      <c r="X48" s="20"/>
+      <c r="Y48" s="20"/>
+      <c r="Z48" s="20"/>
+      <c r="AA48" s="20"/>
+      <c r="AB48" s="20"/>
+      <c r="AC48" s="20"/>
+      <c r="AD48" s="20"/>
+      <c r="AE48" s="20"/>
+      <c r="AF48" s="20"/>
+      <c r="AG48" s="20"/>
+      <c r="AH48" s="20"/>
+      <c r="AI48" s="20"/>
+      <c r="AJ48" s="20"/>
+      <c r="AK48" s="25"/>
+      <c r="AL48" s="25"/>
+      <c r="AM48" s="25"/>
+      <c r="AN48" s="25"/>
+      <c r="AO48" s="25"/>
+      <c r="AP48" s="25"/>
+      <c r="AQ48" s="25"/>
+      <c r="AR48" s="25"/>
+      <c r="AS48" s="25"/>
+      <c r="AT48" s="25"/>
+      <c r="AU48" s="20"/>
+      <c r="AV48" s="20"/>
+      <c r="AW48" s="23"/>
+    </row>
+    <row r="49" spans="1:49">
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="26"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
+      <c r="P49" s="26"/>
+      <c r="Q49" s="26"/>
+      <c r="R49" s="26"/>
+      <c r="S49" s="26"/>
+      <c r="V49" s="18"/>
+      <c r="W49" s="21"/>
+      <c r="X49" s="21"/>
+      <c r="Y49" s="21"/>
+      <c r="Z49" s="21"/>
+      <c r="AA49" s="21"/>
+      <c r="AB49" s="21"/>
+      <c r="AC49" s="21"/>
+      <c r="AD49" s="21"/>
+      <c r="AE49" s="21"/>
+      <c r="AF49" s="21"/>
+      <c r="AG49" s="21"/>
+      <c r="AH49" s="21"/>
+      <c r="AI49" s="21"/>
+      <c r="AJ49" s="21"/>
+      <c r="AK49" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="AL49" s="21"/>
+      <c r="AM49" s="21"/>
+      <c r="AN49" s="21"/>
+      <c r="AO49" s="21"/>
+      <c r="AP49" s="21"/>
+      <c r="AQ49" s="21"/>
+      <c r="AR49" s="21"/>
+      <c r="AS49" s="21"/>
+      <c r="AT49" s="21"/>
+      <c r="AU49" s="21"/>
+      <c r="AV49" s="21"/>
+      <c r="AW49" s="24"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -2928,6 +3534,22 @@
     <mergeCell ref="AL10:AP11"/>
     <mergeCell ref="AQ10:AU11"/>
     <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A39:S39"/>
+    <mergeCell ref="A40:S41"/>
+    <mergeCell ref="Z45:AD45"/>
+    <mergeCell ref="Z47:AD47"/>
+    <mergeCell ref="A42:S42"/>
+    <mergeCell ref="A43:S43"/>
+    <mergeCell ref="A44:S44"/>
+    <mergeCell ref="A45:S45"/>
+    <mergeCell ref="A46:S46"/>
+    <mergeCell ref="A47:S47"/>
+    <mergeCell ref="A48:S48"/>
+    <mergeCell ref="A49:S49"/>
+    <mergeCell ref="V39:AW39"/>
+    <mergeCell ref="V40:AW42"/>
+    <mergeCell ref="AK48:AT48"/>
+    <mergeCell ref="AK49:AT49"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true" horizontalCentered="true"/>
   <pageMargins left="0.472441" right="0.393701" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
grficos: sec y loc ok
</commit_message>
<xml_diff>
--- a/public/Reporte Consolidado Diario.xlsx
+++ b/public/Reporte Consolidado Diario.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>NTS N° 198 - MINSA/DIGESA-2023</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>FERNANDEZ MAURICIO LORENZO</t>
   </si>
   <si>
     <t>SDFSDFDS</t>
@@ -1496,194 +1499,294 @@
         <v>44</v>
       </c>
       <c r="C13" s="10">
+        <v>14</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <f>SUM(L13,P13,T13,X13,AB13,AF13,AJ13,AN13,AS13)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <f>SUM(K13,O13,S13,W13,AA13,AE13,AI13,AM13,AR13)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0</v>
+      </c>
+      <c r="M13" s="10">
+        <v>0</v>
+      </c>
+      <c r="N13" s="10">
+        <v>5</v>
+      </c>
+      <c r="O13" s="10">
+        <v>0</v>
+      </c>
+      <c r="P13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>0</v>
+      </c>
+      <c r="R13" s="10">
+        <v>0</v>
+      </c>
+      <c r="S13" s="10">
+        <v>0</v>
+      </c>
+      <c r="T13" s="10">
+        <v>0</v>
+      </c>
+      <c r="U13" s="10">
+        <v>0</v>
+      </c>
+      <c r="V13" s="10">
+        <v>0</v>
+      </c>
+      <c r="W13" s="10">
+        <v>0</v>
+      </c>
+      <c r="X13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AV13" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="AW13" s="10"/>
+    </row>
+    <row r="14" spans="1:49">
+      <c r="A14" s="13">
+        <v>2</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="10">
         <v>6</v>
       </c>
-      <c r="D13" s="10">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0</v>
-      </c>
-      <c r="F13" s="10">
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
         <v>2</v>
       </c>
-      <c r="G13" s="10">
-        <v>0</v>
-      </c>
-      <c r="H13" s="10">
-        <v>0</v>
-      </c>
-      <c r="I13" s="10">
-        <v>1</v>
-      </c>
-      <c r="J13" s="10">
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <f>SUM(L14,P14,T14,X14,AB14,AF14,AJ14,AN14,AS14)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <f>SUM(K14,O14,S14,W14,AA14,AE14,AI14,AM14,AR14)</f>
+        <v>3</v>
+      </c>
+      <c r="J14" s="10">
         <v>29</v>
       </c>
-      <c r="K13" s="10">
-        <v>0</v>
-      </c>
-      <c r="L13" s="10">
-        <v>0</v>
-      </c>
-      <c r="M13" s="10">
-        <v>0</v>
-      </c>
-      <c r="N13" s="10">
+      <c r="K14" s="10">
+        <v>0</v>
+      </c>
+      <c r="L14" s="10">
+        <v>0</v>
+      </c>
+      <c r="M14" s="10">
+        <v>0</v>
+      </c>
+      <c r="N14" s="10">
         <v>8</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O14" s="10">
         <v>3</v>
       </c>
-      <c r="P13" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="10">
-        <v>0</v>
-      </c>
-      <c r="R13" s="10">
-        <v>0</v>
-      </c>
-      <c r="S13" s="10">
-        <v>0</v>
-      </c>
-      <c r="T13" s="10">
-        <v>0</v>
-      </c>
-      <c r="U13" s="10">
-        <v>0</v>
-      </c>
-      <c r="V13" s="10">
-        <v>0</v>
-      </c>
-      <c r="W13" s="10">
-        <v>0</v>
-      </c>
-      <c r="X13" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AM13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AO13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AP13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AS13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AT13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AU13" s="10">
-        <v>0</v>
-      </c>
-      <c r="AV13" s="10">
+      <c r="P14" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>0</v>
+      </c>
+      <c r="R14" s="10">
+        <v>0</v>
+      </c>
+      <c r="S14" s="10">
+        <v>0</v>
+      </c>
+      <c r="T14" s="10">
+        <v>0</v>
+      </c>
+      <c r="U14" s="10">
+        <v>0</v>
+      </c>
+      <c r="V14" s="10">
+        <v>0</v>
+      </c>
+      <c r="W14" s="10">
+        <v>0</v>
+      </c>
+      <c r="X14" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="10">
         <v>9.0</v>
       </c>
-      <c r="AW13" s="10"/>
-    </row>
-    <row r="14" spans="1:49">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="10"/>
-      <c r="AB14" s="10"/>
-      <c r="AC14" s="10"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="10"/>
-      <c r="AF14" s="10"/>
-      <c r="AG14" s="10"/>
-      <c r="AH14" s="10"/>
-      <c r="AI14" s="10"/>
-      <c r="AJ14" s="10"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="10"/>
-      <c r="AM14" s="10"/>
-      <c r="AN14" s="10"/>
-      <c r="AO14" s="10"/>
-      <c r="AP14" s="10"/>
-      <c r="AQ14" s="10"/>
-      <c r="AR14" s="10"/>
-      <c r="AS14" s="10"/>
-      <c r="AT14" s="10"/>
-      <c r="AU14" s="10"/>
-      <c r="AV14" s="10"/>
       <c r="AW14" s="10"/>
     </row>
     <row r="15" spans="1:49">
@@ -2824,7 +2927,7 @@
       </c>
       <c r="F37" s="13">
         <f>SUM(F13:F36)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G37" s="13">
         <f>SUM(G13:G36)</f>
@@ -2836,7 +2939,7 @@
       </c>
       <c r="I37" s="13">
         <f>SUM(I13:I36)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J37" s="13">
         <f>SUM(J13:J36)</f>
@@ -2856,7 +2959,7 @@
       </c>
       <c r="N37" s="13">
         <f>SUM(N13:N36)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O37" s="13">
         <f>SUM(O13:O36)</f>
@@ -2992,13 +3095,13 @@
       </c>
       <c r="AV37" s="13">
         <f>SUM(AV13:AV36)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="AW37" s="13"/>
     </row>
     <row r="39" spans="1:49">
       <c r="A39" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -3019,7 +3122,7 @@
       <c r="R39" s="15"/>
       <c r="S39" s="15"/>
       <c r="V39" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="W39" s="15"/>
       <c r="X39" s="15"/>
@@ -3051,7 +3154,7 @@
     </row>
     <row r="40" spans="1:49">
       <c r="V40" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:49">
@@ -3252,7 +3355,7 @@
       <c r="R45" s="26"/>
       <c r="S45" s="26"/>
       <c r="V45" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="W45" s="20"/>
       <c r="X45" s="20"/>
@@ -3352,7 +3455,7 @@
       <c r="R47" s="26"/>
       <c r="S47" s="26"/>
       <c r="V47" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W47" s="20"/>
       <c r="X47" s="20"/>
@@ -3467,7 +3570,7 @@
       <c r="AI49" s="21"/>
       <c r="AJ49" s="21"/>
       <c r="AK49" s="30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AL49" s="21"/>
       <c r="AM49" s="21"/>

</xml_diff>